<commit_message>
removed button issues with buildpantry and added timetocook filter
</commit_message>
<xml_diff>
--- a/utils/recipes.xlsx
+++ b/utils/recipes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="300">
   <si>
     <t>title</t>
   </si>
@@ -1134,12 +1134,37 @@
 Stir the chickpea flour and clarified butter together in a saucepan over medium-low heat until the mixture smells toasty, about 10 minutes. Set aside until cool enough to handle.
 Stir in the sugar, pistachios, and cashews until evenly mixed. Form the mixture into small balls the size of large cherries. Use some pressure when forming the balls so they don't come apart.</t>
   </si>
+  <si>
+    <t>Rasgullas</t>
+  </si>
+  <si>
+    <t>"If you are intimidated by the idea of making rasgullas at home, please do not be any longer. I was too, until one day I tried it and realized I was worried for no reason all these years. They are quite easy and super quick to make. Give these a try."</t>
+  </si>
+  <si>
+    <t>https://images.media-allrecipes.com/userphotos/250x250/564413.jpg,https://encrypted-tbn0.gstatic.com/images?q=tbn%3AANd9GcReVDzS5a7OGIQrGskHSvQTVfAJ4ce0iGX8sXUXt2JFLAlSjft7</t>
+  </si>
+  <si>
+    <t>6 cups-milk;3 tablespoons-lime,juiced,fresh;2 1/2 cups-sugar;6 cups-water;1 teaspoon-cardamom,ground</t>
+  </si>
+  <si>
+    <t>1 h 50 m</t>
+  </si>
+  <si>
+    <t>"Prep15 m
+Cook35 m
+Ready In1 h 50 m
+Bring the milk to a boil in a heavy-bottomed pan till it starts foaming; immediately add the lime juice and stir. It will curdle right away. You should see the milk solids (chenna) separate from the whey. Pour into a colander lined with cheesecloth; rinse the chenna with cold water to get rid of the lime juice. Allow the water to drain completely.
+Gather the muslin cloth edges like a parcel and express as much water as possible; what you now have is soft paneer. Turn the paneer onto a rolling mat or other smooth surface. Knead the paneer well to make a smooth paste. Roll into a ball and divide into 20 equal portions.
+Bring the water to a boil in a pressure cooker; stir the sugar into the boiling water until dissolved.
+Roll each portion of paneer into a smooth ball between your palms, making sure there are no cracks; gently drop the balls into the hot syrup. Secure the lid onto the pressure cooker and bring to pressure. Reduce heat to medium-low and pressure cook for 6 minutes.
+Release the pressure from the cooker while running under water; remove the lid. The rasgullas should be floating on the syrup and have expanded 2 or 3 times in size. Pour the rasgullas and syrup into a bowl. Gently stir the cardamom into the mixture. Refrigerate to chill completely before serving cold."</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1182,6 +1207,10 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1211,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1225,10 +1254,13 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1448,7 +1480,8 @@
     <col customWidth="1" min="1" max="1" width="20.5"/>
     <col customWidth="1" min="2" max="2" width="20.13"/>
     <col customWidth="1" min="3" max="3" width="21.5"/>
-    <col customWidth="1" min="4" max="7" width="7.63"/>
+    <col customWidth="1" min="4" max="4" width="75.63"/>
+    <col customWidth="1" min="5" max="7" width="7.63"/>
     <col customWidth="1" min="8" max="8" width="14.5"/>
     <col customWidth="1" min="9" max="9" width="17.88"/>
   </cols>
@@ -1498,7 +1531,7 @@
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1521,13 +1554,13 @@
       <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1550,13 +1583,13 @@
       <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1579,13 +1612,13 @@
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1608,13 +1641,13 @@
       <c r="B6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1637,13 +1670,13 @@
       <c r="B7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1666,13 +1699,13 @@
       <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1695,13 +1728,13 @@
       <c r="B9" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1724,13 +1757,13 @@
       <c r="B10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1753,13 +1786,13 @@
       <c r="B11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1782,13 +1815,13 @@
       <c r="B12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1811,13 +1844,13 @@
       <c r="B13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>85</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1840,13 +1873,13 @@
       <c r="B14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -1869,13 +1902,13 @@
       <c r="B15" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -1898,13 +1931,13 @@
       <c r="B16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -1927,13 +1960,13 @@
       <c r="B17" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -1956,13 +1989,13 @@
       <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>112</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -1985,13 +2018,13 @@
       <c r="B19" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -2014,13 +2047,13 @@
       <c r="B20" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -2043,13 +2076,13 @@
       <c r="B21" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -2072,13 +2105,13 @@
       <c r="B22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -2101,13 +2134,13 @@
       <c r="B23" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="4" t="s">
         <v>139</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -2130,13 +2163,13 @@
       <c r="B24" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>143</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -2159,13 +2192,13 @@
       <c r="B25" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>149</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -2188,13 +2221,13 @@
       <c r="B26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>154</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -2217,13 +2250,13 @@
       <c r="B27" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>159</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -2246,13 +2279,13 @@
       <c r="B28" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>164</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -2275,13 +2308,13 @@
       <c r="B29" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>169</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -2304,7 +2337,7 @@
       <c r="B30" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>174</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -2333,7 +2366,7 @@
       <c r="B31" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>179</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -2362,7 +2395,7 @@
       <c r="B32" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>185</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -2391,7 +2424,7 @@
       <c r="B33" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>190</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -2420,7 +2453,7 @@
       <c r="B34" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>196</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -2449,7 +2482,7 @@
       <c r="B35" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>201</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -2478,7 +2511,7 @@
       <c r="B36" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>207</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -2507,7 +2540,7 @@
       <c r="B37" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>212</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -2536,7 +2569,7 @@
       <c r="B38" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -2565,7 +2598,7 @@
       <c r="B39" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>223</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -2594,7 +2627,7 @@
       <c r="B40" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>229</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -2623,7 +2656,7 @@
       <c r="B41" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>234</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -2652,7 +2685,7 @@
       <c r="B42" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>240</v>
       </c>
       <c r="D42" s="4" t="s">
@@ -2681,7 +2714,7 @@
       <c r="B43" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>245</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -2710,7 +2743,7 @@
       <c r="B44" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>251</v>
       </c>
       <c r="D44" s="5" t="s">
@@ -2739,7 +2772,7 @@
       <c r="B45" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>257</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -2768,7 +2801,7 @@
       <c r="B46" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>262</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -2797,7 +2830,7 @@
       <c r="B47" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>267</v>
       </c>
       <c r="D47" s="4" t="s">
@@ -2826,7 +2859,7 @@
       <c r="B48" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>272</v>
       </c>
       <c r="D48" s="4" t="s">
@@ -2856,7 +2889,7 @@
       <c r="B49" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D49" s="4" t="s">
@@ -2886,7 +2919,7 @@
       <c r="B50" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>285</v>
       </c>
       <c r="D50" s="4" t="s">
@@ -2916,7 +2949,7 @@
       <c r="B51" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>291</v>
       </c>
       <c r="D51" s="4" t="s">
@@ -2940,7 +2973,34 @@
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="H52" s="5"/>
+      <c r="I52" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
@@ -3889,7 +3949,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
@@ -3942,10 +4001,11 @@
     <hyperlink r:id="rId48" ref="C49"/>
     <hyperlink r:id="rId49" ref="C50"/>
     <hyperlink r:id="rId50" ref="C51"/>
+    <hyperlink r:id="rId51" ref="C52"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId51"/>
+  <drawing r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>